<commit_message>
Experiment with finding roads
</commit_message>
<xml_diff>
--- a/Data/Map_coordinates.xlsx
+++ b/Data/Map_coordinates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f7dd912bb4abd67/Maps/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2EC24454-655F-43B1-90B5-D5EB59910066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8DE97C2-48B9-4DCA-916F-DF9F9D4734EF}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="13_ncr:1_{2EC24454-655F-43B1-90B5-D5EB59910066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6434F8D2-0F08-4777-8BE5-5D7F211E2A85}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="870" windowWidth="15900" windowHeight="9330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1830" yWindow="1470" windowWidth="15900" windowHeight="9330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Lat</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Copenhagen</t>
   </si>
   <si>
-    <t>Norway</t>
-  </si>
-  <si>
     <t>Denmark</t>
   </si>
   <si>
@@ -80,6 +77,24 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Puttgarden</t>
+  </si>
+  <si>
+    <t>Rødbyhavn</t>
+  </si>
+  <si>
+    <t>Zealand</t>
+  </si>
+  <si>
+    <t>Lolland</t>
+  </si>
+  <si>
+    <t>Area</t>
   </si>
 </sst>
 </file>
@@ -123,10 +138,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -454,7 +470,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -463,189 +479,245 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>55.674710841822602</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12.5479546156857</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>55.604871842410702</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12.998803670956001</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>55.476598985594599</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8.46347610478478</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
+        <v>55.405194838905501</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10.3978091119127</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1">
+        <v>54.795085825307098</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9.44890142501559</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1">
+        <v>53.864289589843402</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10.686520488613899</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>53.552870721352498</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9.9838571232206093</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>54.091901975413997</v>
+      </c>
+      <c r="C9" s="1">
+        <v>12.0975041855441</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>54.130948357757099</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11.3009213794648</v>
+      </c>
+      <c r="D10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1">
-        <v>55.676111111110998</v>
-      </c>
-      <c r="C2" s="1">
-        <v>12.568888888888999</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>55.603313100000001</v>
-      </c>
-      <c r="C3" s="1">
-        <v>13.0013112</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1">
-        <v>55.29</v>
-      </c>
-      <c r="C4" s="1">
-        <v>8.27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1">
-        <v>55.23</v>
-      </c>
-      <c r="C5" s="1">
-        <v>10.23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1">
-        <v>54.46</v>
-      </c>
-      <c r="C6" s="1">
-        <v>9.26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1">
-        <v>53.869624100000003</v>
-      </c>
-      <c r="C7" s="1">
-        <v>10.6875868</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1">
-        <v>53.533200000000001</v>
-      </c>
-      <c r="C8" s="1">
-        <v>10.005000000000001</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1">
-        <v>54.5</v>
-      </c>
-      <c r="C9" s="1">
-        <v>12.8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1">
-        <v>58.633000000000003</v>
-      </c>
-      <c r="C10" s="1">
-        <v>19.431000000000001</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>55.641492857633502</v>
+      </c>
+      <c r="C11" s="1">
+        <v>13.817589171098</v>
+      </c>
+      <c r="D11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>55.672266880016103</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9.6936255879641298</v>
+      </c>
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>62.74</v>
-      </c>
-      <c r="C11" s="1">
-        <v>15.52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1">
-        <v>61.93</v>
-      </c>
-      <c r="C12" s="1">
-        <v>9.24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
       <c r="B13" s="1">
-        <v>55.58</v>
+        <v>54.2811112753527</v>
       </c>
       <c r="C13" s="1">
-        <v>10.130000000000001</v>
+        <v>7.6891929728222896</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>10</v>
+      <c r="A14" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B14" s="1">
-        <v>56.4</v>
+        <v>53.999009455232702</v>
       </c>
       <c r="C14" s="1">
-        <v>5.21</v>
+        <v>12.806216587324201</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1">
+        <v>54.496764791930801</v>
+      </c>
+      <c r="C15" s="1">
+        <v>11.211642658493</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>54.665869430700802</v>
+      </c>
+      <c r="C16" s="1">
+        <v>11.3447334080702</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1">
+        <v>55.422816329253997</v>
+      </c>
+      <c r="C17" s="1">
+        <v>11.922727341180501</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1">
+        <v>54.8712804655433</v>
+      </c>
+      <c r="C18" s="1">
+        <v>11.4588207589163</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>